<commit_message>
fix export data absen pegawai
</commit_message>
<xml_diff>
--- a/directory/templates/template-absensi-pegawai.xlsx
+++ b/directory/templates/template-absensi-pegawai.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\hrmis\directory\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\hrmis-master\directory\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383CF24D-3B48-44FB-9F49-D3516FA65A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20D9613-B75E-4E0C-84E0-9F792E6B64E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{31A0B364-D528-4097-98D0-DBAC8A79801F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{31A0B364-D528-4097-98D0-DBAC8A79801F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -335,7 +335,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -401,14 +401,20 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -428,14 +434,11 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -781,42 +784,42 @@
   <dimension ref="A1:Z13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" customWidth="1"/>
-    <col min="5" max="5" width="4.6640625" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" customWidth="1"/>
-    <col min="9" max="9" width="4.6640625" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="12"/>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
@@ -830,21 +833,21 @@
       <c r="Y1" s="5"/>
       <c r="Z1" s="6"/>
     </row>
-    <row r="2" spans="1:26" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="12"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
@@ -858,7 +861,7 @@
       <c r="Y2" s="5"/>
       <c r="Z2" s="6"/>
     </row>
-    <row r="3" spans="1:26" ht="21.6" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="21.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -871,8 +874,8 @@
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
       <c r="O3" s="7"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
@@ -886,12 +889,12 @@
       <c r="Y3" s="7"/>
       <c r="Z3" s="6"/>
     </row>
-    <row r="4" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="32"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="24" t="s">
         <v>16</v>
       </c>
@@ -903,8 +906,8 @@
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
@@ -918,12 +921,12 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="6"/>
     </row>
-    <row r="5" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="33"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="24" t="s">
         <v>18</v>
       </c>
@@ -935,8 +938,8 @@
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
@@ -950,12 +953,12 @@
       <c r="Y5" s="7"/>
       <c r="Z5" s="6"/>
     </row>
-    <row r="6" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="32"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="24" t="s">
         <v>23</v>
       </c>
@@ -967,8 +970,8 @@
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
@@ -982,12 +985,12 @@
       <c r="Y6" s="7"/>
       <c r="Z6" s="6"/>
     </row>
-    <row r="7" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="33"/>
+      <c r="C7" s="35"/>
       <c r="D7" s="24" t="s">
         <v>24</v>
       </c>
@@ -999,8 +1002,8 @@
       <c r="J7" s="15"/>
       <c r="K7" s="22"/>
       <c r="L7" s="22"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
@@ -1014,12 +1017,12 @@
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
     </row>
-    <row r="8" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="33"/>
+      <c r="C8" s="35"/>
       <c r="D8" s="24" t="s">
         <v>25</v>
       </c>
@@ -1031,8 +1034,8 @@
       <c r="J8" s="16"/>
       <c r="K8" s="16"/>
       <c r="L8" s="23"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
@@ -1046,7 +1049,7 @@
       <c r="Y8" s="8"/>
       <c r="Z8" s="6"/>
     </row>
-    <row r="9" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
@@ -1059,8 +1062,8 @@
       <c r="J9" s="16"/>
       <c r="K9" s="16"/>
       <c r="L9" s="22"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
@@ -1074,33 +1077,33 @@
       <c r="Y9" s="9"/>
       <c r="Z9" s="6"/>
     </row>
-    <row r="10" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34" t="s">
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="25" t="s">
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="25" t="s">
+      <c r="M10" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="N10" s="11"/>
+      <c r="N10" s="36"/>
       <c r="O10" s="11"/>
       <c r="P10" s="11"/>
       <c r="Q10" s="11"/>
@@ -1114,34 +1117,35 @@
       <c r="Y10" s="11"/>
       <c r="Z10" s="6"/>
     </row>
-    <row r="11" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="34" t="s">
+      <c r="B11" s="32"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="34"/>
+      <c r="E11" s="27"/>
       <c r="F11" s="17" t="s">
         <v>7</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="34" t="s">
+      <c r="H11" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="34"/>
+      <c r="I11" s="27"/>
       <c r="J11" s="17" t="s">
         <v>7</v>
       </c>
       <c r="K11" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="16"/>
     </row>
-    <row r="12" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="19" t="s">
         <v>1</v>
@@ -1149,10 +1153,10 @@
       <c r="C12" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="36" t="s">
+      <c r="E12" s="26" t="s">
         <v>26</v>
       </c>
       <c r="F12" s="20" t="s">
@@ -1161,10 +1165,10 @@
       <c r="G12" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="35" t="s">
+      <c r="H12" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="36" t="s">
+      <c r="I12" s="26" t="s">
         <v>28</v>
       </c>
       <c r="J12" s="20" t="s">
@@ -1179,8 +1183,9 @@
       <c r="M12" s="21" t="s">
         <v>31</v>
       </c>
+      <c r="N12" s="16"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -1193,16 +1198,11 @@
       <c r="J13" s="16"/>
       <c r="K13" s="16"/>
       <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B1:K2"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="B4:C4"/>
@@ -1210,17 +1210,14 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B1:M2"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="H11:I11"/>
   </mergeCells>
-  <conditionalFormatting sqref="E10:E12">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I10:I12">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>